<commit_message>
updated run of data clean and merge
</commit_message>
<xml_diff>
--- a/species_lists/KEEN ONE New England Species List v1.3.4.xlsx
+++ b/species_lists/KEEN ONE New England Species List v1.3.4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Complete_GOM_Taxa" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="798">
   <si>
     <t>sea cauliflower</t>
   </si>
@@ -2518,6 +2518,12 @@
   </si>
   <si>
     <t>We use WORMS for all taxonomy</t>
+  </si>
+  <si>
+    <t>CAMS</t>
+  </si>
+  <si>
+    <t>Fixed carcinus maenas juvennile problem</t>
   </si>
 </sst>
 </file>
@@ -2704,7 +2710,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="182">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2789,6 +2795,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3149,7 +3156,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="182">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3289,6 +3296,7 @@
     <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3660,8 +3668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C66" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView topLeftCell="C93" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7156,7 +7164,7 @@
     <row r="114" spans="1:44">
       <c r="B114" s="3"/>
       <c r="D114" s="46" t="s">
-        <v>737</v>
+        <v>796</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>324</v>
@@ -10364,9 +10372,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -10576,6 +10584,17 @@
       </c>
       <c r="C20" t="s">
         <v>793</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="35">
+        <v>41459</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>788</v>
+      </c>
+      <c r="C21" t="s">
+        <v>797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>